<commit_message>
update model version lable
</commit_message>
<xml_diff>
--- a/INPUT_OUTPUT_FILES/3D_CMCC_FEM_Settings_template.xlsx
+++ b/INPUT_OUTPUT_FILES/3D_CMCC_FEM_Settings_template.xlsx
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="197">
   <si>
     <t xml:space="preserve">SETTING PARAMETERS LIST for THE MODEL 3D-CMCC-FEM </t>
   </si>
@@ -95,6 +95,9 @@
     <t xml:space="preserve">5.5-ISIMIP</t>
   </si>
   <si>
+    <t xml:space="preserve">5.6.06</t>
+  </si>
+  <si>
     <t xml:space="preserve">SITENAME</t>
   </si>
   <si>
@@ -312,6 +315,9 @@
   </si>
   <si>
     <t xml:space="preserve">when on, GPP follows a cold-acclimation (usefull in boreal areas)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">not activated in 5.6</t>
   </si>
   <si>
     <t xml:space="preserve">N_REG</t>
@@ -958,10 +964,10 @@
   </sheetPr>
   <dimension ref="A1:I74"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1380" topLeftCell="A1" activePane="bottomLeft" state="split"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+      <selection pane="bottomLeft" activeCell="L7" activeCellId="0" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1045,8 +1051,8 @@
       <c r="G5" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="14" t="n">
-        <v>5.6</v>
+      <c r="H5" s="14" t="s">
+        <v>13</v>
       </c>
       <c r="I5" s="14" t="n">
         <v>5.7</v>
@@ -1054,1606 +1060,1610 @@
     </row>
     <row r="6" customFormat="false" ht="25.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B6" s="15"/>
       <c r="C6" s="16" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D6" s="16"/>
       <c r="E6" s="15" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F6" s="17"/>
       <c r="G6" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="25.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F7" s="20" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G7" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="25.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F8" s="20" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G8" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="25.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F9" s="20" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="25.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F10" s="20" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G10" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="25.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B11" s="19" t="n">
         <v>6000</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F11" s="20"/>
       <c r="G11" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="25.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B12" s="15"/>
       <c r="C12" s="16" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F12" s="20"/>
       <c r="G12" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="25.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B13" s="15"/>
       <c r="C13" s="16" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F13" s="20"/>
       <c r="G13" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="25.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B14" s="15"/>
       <c r="C14" s="16" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D14" s="16"/>
       <c r="E14" s="15" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F14" s="17"/>
       <c r="G14" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="25.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B15" s="15"/>
       <c r="C15" s="16" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D15" s="16"/>
       <c r="E15" s="15" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F15" s="17"/>
       <c r="G15" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="25.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B16" s="15"/>
       <c r="C16" s="16" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D16" s="16"/>
       <c r="E16" s="15" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F16" s="20"/>
       <c r="G16" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="25.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E17" s="15"/>
       <c r="F17" s="20"/>
       <c r="G17" s="18"/>
       <c r="I17" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="25.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D18" s="16" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E18" s="15" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F18" s="20"/>
       <c r="G18" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H18" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I18" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="25.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C19" s="16" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D19" s="16" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E19" s="15" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F19" s="20" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G19" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H19" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I19" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="25.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B20" s="15"/>
       <c r="C20" s="16" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D20" s="16"/>
       <c r="E20" s="15" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F20" s="17"/>
       <c r="G20" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H20" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I20" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="25.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B21" s="15"/>
       <c r="C21" s="16" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D21" s="16"/>
       <c r="E21" s="15" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F21" s="17"/>
       <c r="G21" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H21" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I21" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="25.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D22" s="16" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E22" s="15" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F22" s="20" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G22" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H22" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I22" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="25.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B23" s="15"/>
       <c r="C23" s="16" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D23" s="16" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E23" s="15" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F23" s="20"/>
       <c r="G23" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H23" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I23" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="25.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B24" s="15"/>
       <c r="C24" s="16" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D24" s="16" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E24" s="15" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F24" s="20" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G24" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H24" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I24" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="25.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B25" s="19" t="n">
         <v>-9999</v>
       </c>
       <c r="C25" s="16" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D25" s="16"/>
       <c r="E25" s="15" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F25" s="20"/>
       <c r="G25" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H25" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I25" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="25.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C26" s="16" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D26" s="16" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E26" s="15" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F26" s="20"/>
       <c r="G26" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H26" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I26" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="25.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B27" s="15"/>
       <c r="C27" s="16" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D27" s="16" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E27" s="15" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F27" s="20"/>
       <c r="G27" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H27" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I27" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="25.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B28" s="15"/>
       <c r="C28" s="16" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D28" s="16" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E28" s="15" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F28" s="20"/>
       <c r="G28" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H28" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I28" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="25.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B29" s="15"/>
       <c r="C29" s="16" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D29" s="16" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E29" s="15"/>
-      <c r="F29" s="20"/>
+      <c r="F29" s="20" t="s">
+        <v>87</v>
+      </c>
       <c r="G29" s="18"/>
       <c r="H29" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I29" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="25.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B30" s="15"/>
       <c r="C30" s="16" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D30" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="E30" s="15"/>
+      <c r="F30" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="E30" s="15"/>
-      <c r="F30" s="20"/>
       <c r="G30" s="18"/>
       <c r="H30" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I30" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="25.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B31" s="15"/>
       <c r="C31" s="16" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D31" s="16" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="E31" s="15" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F31" s="20"/>
       <c r="G31" s="18"/>
       <c r="H31" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I31" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="25.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B32" s="15"/>
       <c r="C32" s="16" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D32" s="21"/>
       <c r="E32" s="15" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F32" s="16" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="G32" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H32" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I32" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="25.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B33" s="15"/>
       <c r="C33" s="16" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D33" s="21" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="E33" s="15"/>
       <c r="F33" s="16"/>
       <c r="G33" s="18"/>
       <c r="I33" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="25.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B34" s="15"/>
       <c r="C34" s="16" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D34" s="16" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E34" s="15" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F34" s="16" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="G34" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H34" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I34" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="25.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B35" s="19" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C35" s="16" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="D35" s="16"/>
       <c r="E35" s="15" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F35" s="16"/>
       <c r="G35" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H35" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I35" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="25.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B36" s="15"/>
       <c r="C36" s="16" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D36" s="16" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="E36" s="15" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="F36" s="16" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="G36" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H36" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I36" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="25.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B37" s="19" t="n">
         <v>0.48</v>
       </c>
       <c r="C37" s="16" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="D37" s="16"/>
       <c r="E37" s="15" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F37" s="16"/>
       <c r="G37" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H37" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I37" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="25.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B38" s="19" t="n">
         <v>368.865</v>
       </c>
       <c r="C38" s="16" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="D38" s="16"/>
       <c r="E38" s="15" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="F38" s="22" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="G38" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H38" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I38" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="25.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B39" s="19" t="n">
         <v>0.01</v>
       </c>
       <c r="C39" s="16" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="D39" s="16"/>
       <c r="E39" s="15" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F39" s="16" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="G39" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H39" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I39" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="25.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B40" s="19" t="n">
         <v>1</v>
       </c>
       <c r="C40" s="16" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="D40" s="16"/>
       <c r="E40" s="15" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="F40" s="16"/>
       <c r="G40" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H40" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I40" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="25.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B41" s="19" t="n">
         <v>3</v>
       </c>
       <c r="C41" s="16" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="D41" s="16"/>
       <c r="E41" s="15" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="F41" s="16" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="G41" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H41" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I41" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="25.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B42" s="19" t="n">
         <v>1</v>
       </c>
       <c r="C42" s="16" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="D42" s="16" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="E42" s="15" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F42" s="20"/>
       <c r="G42" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H42" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I42" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="25.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B43" s="19" t="n">
         <v>1.2</v>
       </c>
       <c r="C43" s="16" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="D43" s="16"/>
       <c r="E43" s="15"/>
       <c r="F43" s="15"/>
       <c r="G43" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H43" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I43" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="25.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B44" s="20"/>
       <c r="C44" s="16" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="D44" s="16" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="E44" s="15" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F44" s="16" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="G44" s="18"/>
       <c r="I44" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="25.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B45" s="20"/>
       <c r="C45" s="16" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="E45" s="15" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="F45" s="16"/>
       <c r="G45" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H45" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I45" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="25.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B46" s="15"/>
       <c r="C46" s="16" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="D46" s="16"/>
       <c r="E46" s="15" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F46" s="20"/>
       <c r="G46" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H46" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I46" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="25.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B47" s="15"/>
       <c r="C47" s="16" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="D47" s="16" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="E47" s="15" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F47" s="20" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="G47" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H47" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I47" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="25.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B48" s="15"/>
       <c r="C48" s="16" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D48" s="16"/>
       <c r="E48" s="15" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="F48" s="20"/>
       <c r="G48" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H48" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I48" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="25.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B49" s="15"/>
       <c r="C49" s="16" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="D49" s="16"/>
       <c r="E49" s="15" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F49" s="20"/>
       <c r="G49" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H49" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I49" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="25.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B50" s="15"/>
       <c r="C50" s="16" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="D50" s="16"/>
       <c r="E50" s="15" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="F50" s="20"/>
       <c r="G50" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H50" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I50" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="25.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B51" s="19" t="n">
         <v>-9999</v>
       </c>
       <c r="C51" s="16" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="D51" s="16"/>
       <c r="E51" s="15" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="F51" s="15" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G51" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H51" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I51" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="25.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B52" s="15"/>
       <c r="C52" s="16" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="D52" s="16"/>
       <c r="E52" s="15" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="F52" s="20"/>
       <c r="G52" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H52" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I52" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="25.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B53" s="19" t="n">
         <v>0</v>
       </c>
       <c r="C53" s="16" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="D53" s="16"/>
       <c r="E53" s="15" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="F53" s="15"/>
       <c r="G53" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H53" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I53" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="25.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B54" s="19" t="n">
         <v>0</v>
       </c>
       <c r="C54" s="16" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="D54" s="16"/>
       <c r="E54" s="15" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="F54" s="15"/>
       <c r="G54" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H54" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I54" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="25.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B55" s="19" t="n">
         <v>0</v>
       </c>
       <c r="C55" s="16" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="D55" s="16"/>
       <c r="E55" s="15" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="F55" s="15"/>
       <c r="G55" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H55" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I55" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="25.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="B56" s="19" t="n">
         <v>0</v>
       </c>
       <c r="C56" s="16" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="D56" s="16"/>
       <c r="E56" s="15" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="F56" s="15"/>
       <c r="G56" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H56" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I56" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="25.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B57" s="19" t="n">
         <v>0</v>
       </c>
       <c r="C57" s="16" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="D57" s="16"/>
       <c r="E57" s="15" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="F57" s="15"/>
       <c r="G57" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H57" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I57" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="25.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B58" s="19" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C58" s="16" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="D58" s="16" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="E58" s="15" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F58" s="15" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="G58" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="25.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B59" s="19" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="C59" s="16" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="D59" s="16"/>
       <c r="E59" s="15" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F59" s="15" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="G59" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="25.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B60" s="19" t="n">
         <v>-9999</v>
       </c>
       <c r="C60" s="16" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="D60" s="16"/>
       <c r="E60" s="15" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="F60" s="15" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="G60" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="25.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B61" s="19" t="n">
         <v>1</v>
       </c>
       <c r="C61" s="16" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="D61" s="16"/>
       <c r="E61" s="15" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F61" s="15" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="G61" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="25.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B62" s="19" t="n">
         <v>0.1</v>
       </c>
       <c r="C62" s="16" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="D62" s="16"/>
       <c r="E62" s="15" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="F62" s="15" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="G62" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="25.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B63" s="19" t="n">
         <v>0</v>
       </c>
       <c r="C63" s="16" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="D63" s="16"/>
       <c r="E63" s="15" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="F63" s="15" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="G63" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="25.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B64" s="19" t="n">
         <v>1.2</v>
       </c>
       <c r="C64" s="16" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="D64" s="16"/>
       <c r="E64" s="15" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="F64" s="15" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="G64" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="25.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="B65" s="19" t="n">
         <v>0</v>
       </c>
       <c r="C65" s="16" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="D65" s="16"/>
       <c r="E65" s="15" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="F65" s="15" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="G65" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="25.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B66" s="19" t="n">
         <v>0</v>
       </c>
       <c r="C66" s="16" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="D66" s="16"/>
       <c r="E66" s="15" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="F66" s="15" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="G66" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="25.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B67" s="19" t="n">
         <v>0</v>
       </c>
       <c r="C67" s="16" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="D67" s="16"/>
       <c r="E67" s="15" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="F67" s="15" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="G67" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="25.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B68" s="19" t="n">
         <v>0</v>
       </c>
       <c r="C68" s="16" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="D68" s="16"/>
       <c r="E68" s="15" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="F68" s="15" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="G68" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="25.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="B69" s="19" t="n">
         <v>0</v>
       </c>
       <c r="C69" s="16" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="D69" s="16"/>
       <c r="E69" s="15" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="F69" s="15" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="G69" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="25.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="B70" s="19" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C70" s="16" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D70" s="16" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="E70" s="15" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F70" s="15"/>
       <c r="G70" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H70" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I70" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="25.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B71" s="19" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C71" s="16" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D71" s="16" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="E71" s="15" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F71" s="15"/>
       <c r="G71" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H71" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I71" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="25.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>